<commit_message>
added remaining fishes to fish_desc
</commit_message>
<xml_diff>
--- a/fish_desc.xlsx
+++ b/fish_desc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kik\Documents\GitHub\argo_ocean_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5A3B07-980C-4D95-80C2-72851221700D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704ADDCA-9731-4506-ABFE-3D8767D18726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>fish_name</t>
   </si>
@@ -44,9 +44,6 @@
     <t>https://upload.wikimedia.org/wikipedia/commons/3/30/Pollachius_virens.png</t>
   </si>
   <si>
-    <t>Pollock</t>
-  </si>
-  <si>
     <t>fishbase_link</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>37 - 364 m</t>
   </si>
   <si>
-    <t>Sand lance</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=3822&amp;AT=Sand%20lances</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>https://ogsl.ca/app-guidespeces/action/AffichageImage?typeImg=espece&amp;id=117&amp;h=700&amp;l=700</t>
   </si>
   <si>
-    <t>White barracudina</t>
-  </si>
-  <si>
     <t>0 - 2200 m</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>https://mare.istc.cnr.it/fisheriesv2/javax.faces.resource/pictograms/argentina_silus.jpg.xhtml?ln=images</t>
   </si>
   <si>
-    <t>Atlantic argentine</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=2700&amp;AT=atlantic+argentine</t>
   </si>
   <si>
@@ -113,9 +101,6 @@
     <t>https://alchetron.com/cdn/arctogadus-glacialis-76112ffc-1930-4e9f-b1c7-41d0a632c7a-resize-750.jpeg</t>
   </si>
   <si>
-    <t>Arctic cod</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=1872&amp;AT=arctic+cod</t>
   </si>
   <si>
@@ -128,9 +113,6 @@
     <t>https://upload.wikimedia.org/wikipedia/commons/0/04/Clupea_harengus.png</t>
   </si>
   <si>
-    <t>Atlantic herring</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=24&amp;AT=atlantic+herring</t>
   </si>
   <si>
@@ -143,9 +125,6 @@
     <t>https://i.pinimg.com/originals/2f/23/f9/2f23f9bd997e4c1a2b7439c79b9fa67d.jpg</t>
   </si>
   <si>
-    <t>Lumpfish</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=62&amp;AT=lumpfish</t>
   </si>
   <si>
@@ -158,9 +137,6 @@
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=2420&amp;AT=threespine+stickleback</t>
   </si>
   <si>
-    <t>Three-spined stickleback</t>
-  </si>
-  <si>
     <t>https://nas.er.usgs.gov/XIMAGESERVERX/2019/20190506121725.jpg</t>
   </si>
   <si>
@@ -173,9 +149,6 @@
     <t>https://www.newsea.dk/media/zoo/images/Capelin_Mallotus-villosus_d5f220b832d079606caf3ce8eec94e2d.png</t>
   </si>
   <si>
-    <t>Capelin</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=252&amp;AT=capelin</t>
   </si>
   <si>
@@ -183,16 +156,87 @@
   </si>
   <si>
     <t>Oceanic species found in schools. Nerito-pelagic. Adults feed on planktonic crustaceans, copepods, euphausiids, amphipods, marine worms, and small fishes. Mature individuals move inshore in large schools to spawn. In the spring large spawning shoals migrate toward the coasts, males usually arrive first. Often entering brackish and freshwaters. </t>
+  </si>
+  <si>
+    <t>picture_credits</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=253&amp;AT=rainbow+smelt</t>
+  </si>
+  <si>
+    <t>rainbow smelt</t>
+  </si>
+  <si>
+    <t>pollock</t>
+  </si>
+  <si>
+    <t>sand lance</t>
+  </si>
+  <si>
+    <t>white barracudina</t>
+  </si>
+  <si>
+    <t>atlantic argentine</t>
+  </si>
+  <si>
+    <t>arctic cod</t>
+  </si>
+  <si>
+    <t>atlantic herring</t>
+  </si>
+  <si>
+    <t>lumpfish</t>
+  </si>
+  <si>
+    <t>three-spined stickleback</t>
+  </si>
+  <si>
+    <t>capelin</t>
+  </si>
+  <si>
+    <t>0 - 425 m</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/proxy/fWp65SuSmwvlvwEj26IR4izegVP75gEWHVt9Pd_1xi5ejc2hlVzfqHFzS6yMXxWd8W7NOGur21sJ0XDlq5RIaOK-eR2fWapDe_9sr_kIMnZpUYsPaXgWvFSMI-rYjgaDIMcPTMGnTZRKdOuJSTezzWhTShM</t>
+  </si>
+  <si>
+    <t>Nerito-pelagic. Inhabits cool clear lakes, medium to large rivers, and coastal waters. A schooling species that occurs in midwater of lakes or inshore coastal waters; at temperatures ranging from 7.2-15.6°C. Coastal population are anadromous. Migrates up to 1,000 km upstream in rivers. Feeds on invertebrates such as amphipods, ostracods, aquatic insect larvae and aquatic worms; food also include copepods, euphausiids, mysids and small fishes (silversides, mummichogs and herring).</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=3150&amp;AT=atlantic+soft+pout</t>
+  </si>
+  <si>
+    <t>atlantic soft pout</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/images/species/Meatl_u0.jpg</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/Collaborators/CollaboratorSummary.php?ID=268</t>
+  </si>
+  <si>
+    <t>400 - 1853 m</t>
+  </si>
+  <si>
+    <t>Occurs in midwater over the continental slope. Mostly found from 365-550 m depth, but enters shallower water in the northern part of range; prefers salinity of 33.4-34.7 ppt. Bathypelagic. Feeds on foraminifera, copepods, and ostracods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,15 +259,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,15 +583,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47884F28-8B4B-4CA1-A41B-DBA99BFEDAA0}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,170 +605,213 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{F1773C53-AD19-4A19-B711-E886B844EEA9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added misshing silver hake
</commit_message>
<xml_diff>
--- a/fish_desc.xlsx
+++ b/fish_desc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kik\Documents\GitHub\argo_ocean_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704ADDCA-9731-4506-ABFE-3D8767D18726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6E10F2-138B-48B0-9A47-AB29A27043BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>fish_name</t>
   </si>
@@ -219,6 +219,39 @@
   </si>
   <si>
     <t>Occurs in midwater over the continental slope. Mostly found from 365-550 m depth, but enters shallower water in the northern part of range; prefers salinity of 33.4-34.7 ppt. Bathypelagic. Feeds on foraminifera, copepods, and ostracods</t>
+  </si>
+  <si>
+    <t>Flescher, Don</t>
+  </si>
+  <si>
+    <t>credits_link</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/File:Pollachius_virens.png</t>
+  </si>
+  <si>
+    <t>Wikimedia Commons</t>
+  </si>
+  <si>
+    <t>Theresa Liedtke</t>
+  </si>
+  <si>
+    <t>https://www.usgs.gov/media/images/pacific-sand-lance</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=323&amp;AT=silver+hake</t>
+  </si>
+  <si>
+    <t>silver hake</t>
+  </si>
+  <si>
+    <t>https://www.conxemar.com/sites/conxemar/files/merluccius_bilinearis_sw.jpeg</t>
+  </si>
+  <si>
+    <t>55 - 914 m </t>
+  </si>
+  <si>
+    <t>Abundant on sandy grounds and strays into shallower waters. A voracious predator with cannibalistic habits. Individuals over 40 cm TL prey on fishes such as gadoids and herring, while smaller ones feed on crustaceans, i.e. euphausiids and pandalids; food also includes gaspereau, myctophids, smelt, silversides, mackerel, sand lance, butterfish, snakeblennies, longhorn sculpins and squids. The smallest specimen feeds mostly on crustaceans (Ref. 58452).</t>
   </si>
 </sst>
 </file>
@@ -583,21 +616,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47884F28-8B4B-4CA1-A41B-DBA99BFEDAA0}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="2" max="4" width="36" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,186 +641,201 @@
         <v>41</v>
       </c>
       <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
       <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>55</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -795,23 +843,47 @@
         <v>58</v>
       </c>
       <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>61</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{F1773C53-AD19-4A19-B711-E886B844EEA9}"/>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{F1773C53-AD19-4A19-B711-E886B844EEA9}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{8317E9C9-1A1E-48E5-89C6-6E10BAE0D98F}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{3DEDF7B5-7AF5-42B1-96C5-B61C6B9D5CFB}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{6B23C7F8-DD8E-4996-939A-94246C59B42E}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{E63DF56C-245A-48AF-81A3-4014B3F250E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added image credits to all fishes
</commit_message>
<xml_diff>
--- a/fish_desc.xlsx
+++ b/fish_desc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kik\Documents\GitHub\argo_ocean_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6E10F2-138B-48B0-9A47-AB29A27043BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22B5AC0-44EB-42FC-A90F-D3E94A6EAF89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>fish_name</t>
   </si>
@@ -74,9 +74,6 @@
     <t>May occur in large schools near the surface both inshore and offshore, but also buries itself in sand. Inshore, found from intertidal to subtidal areas. Offshore, found near the surface over deep water. Benthic. Juveniles and adults feed on zooplankton.</t>
   </si>
   <si>
-    <t>https://ogsl.ca/app-guidespeces/action/AffichageImage?typeImg=espece&amp;id=117&amp;h=700&amp;l=700</t>
-  </si>
-  <si>
     <t>0 - 2200 m</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Pseudoceanic and mesopelagic, occurring singly or in small schools, primarily at 200-1000m. Feed mainly on fishes and shrimps. Spawn in continental slopes and in oceanic banks from northern through tropical to southern temperate waters. Oviparous, with planktonic larvae </t>
   </si>
   <si>
-    <t>https://mare.istc.cnr.it/fisheriesv2/javax.faces.resource/pictograms/argentina_silus.jpg.xhtml?ln=images</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=2700&amp;AT=atlantic+argentine</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>Bathypelagic. Prefer depths of 182.8-255.9 m, temperature 7-10°C and mean salinity 34 ppt. Probably form schools close to the bottom. Feeds on planktonic invertebrates including euphausiids, amphipods (arrow worms, krill and Thermisto), chaetognaths, squids and ctenophores, also small fishes. Spawns from April to July. Growth is slow. Eggs and young are pelagic at depths of 400-500m.</t>
   </si>
   <si>
-    <t>https://alchetron.com/cdn/arctogadus-glacialis-76112ffc-1930-4e9f-b1c7-41d0a632c7a-resize-750.jpeg</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=1872&amp;AT=arctic+cod</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>Herring schools move between spawning and wintering grounds in coastal areas and feeding grounds in open water by following migration patterns learned from earlier year classes. Juveniles (up to 2 years) shoal close inshore, while adults are found more offshore. Adults spend the day in deeper water, but rise to shallower water at night. Light is an important factor in controlling their vertical distribution. Feed mainly on copepods finding food by visual sense.</t>
   </si>
   <si>
-    <t>https://i.pinimg.com/originals/2f/23/f9/2f23f9bd997e4c1a2b7439c79b9fa67d.jpg</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=62&amp;AT=lumpfish</t>
   </si>
   <si>
@@ -146,9 +134,6 @@
     <t>Adults occur in fresh waters, estuaries and coastal seas. Anadromous, with numerous non-anadromous populations in brackish or pure freshwater, rarely in marine waters. In the sea, confined to coastal waters. In freshwater, adults prefer to live in small stream but may occur in a variety of habitats including lakes and large rivers. Inhabit shallow vegetated areas, usually over mud or sand. Form schools. Young associated with drifting seaweed. Juveniles move to the sea (anadromous populations) or to deeper, larger water bodies (freshwater populations) in July-August, forming large feeding schools. Feed on worms, crustaceans, larvae and adult aquatic insects, drowned aerial insects, and small fishes; has also been reported to feed on their own fry and eggs. Eggs are found in nests constructed from plant material. Males build, guard and aerate the nest where the eggs are deposited.</t>
   </si>
   <si>
-    <t>https://www.newsea.dk/media/zoo/images/Capelin_Mallotus-villosus_d5f220b832d079606caf3ce8eec94e2d.png</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=252&amp;AT=capelin</t>
   </si>
   <si>
@@ -188,18 +173,12 @@
     <t>lumpfish</t>
   </si>
   <si>
-    <t>three-spined stickleback</t>
-  </si>
-  <si>
     <t>capelin</t>
   </si>
   <si>
     <t>0 - 425 m</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/proxy/fWp65SuSmwvlvwEj26IR4izegVP75gEWHVt9Pd_1xi5ejc2hlVzfqHFzS6yMXxWd8W7NOGur21sJ0XDlq5RIaOK-eR2fWapDe_9sr_kIMnZpUYsPaXgWvFSMI-rYjgaDIMcPTMGnTZRKdOuJSTezzWhTShM</t>
-  </si>
-  <si>
     <t>Nerito-pelagic. Inhabits cool clear lakes, medium to large rivers, and coastal waters. A schooling species that occurs in midwater of lakes or inshore coastal waters; at temperatures ranging from 7.2-15.6°C. Coastal population are anadromous. Migrates up to 1,000 km upstream in rivers. Feeds on invertebrates such as amphipods, ostracods, aquatic insect larvae and aquatic worms; food also include copepods, euphausiids, mysids and small fishes (silversides, mummichogs and herring).</t>
   </si>
   <si>
@@ -245,20 +224,104 @@
     <t>silver hake</t>
   </si>
   <si>
-    <t>https://www.conxemar.com/sites/conxemar/files/merluccius_bilinearis_sw.jpeg</t>
-  </si>
-  <si>
     <t>55 - 914 m </t>
   </si>
   <si>
     <t>Abundant on sandy grounds and strays into shallower waters. A voracious predator with cannibalistic habits. Individuals over 40 cm TL prey on fishes such as gadoids and herring, while smaller ones feed on crustaceans, i.e. euphausiids and pandalids; food also includes gaspereau, myctophids, smelt, silversides, mackerel, sand lance, butterfish, snakeblennies, longhorn sculpins and squids. The smallest specimen feeds mostly on crustaceans (Ref. 58452).</t>
+  </si>
+  <si>
+    <t>https://fishesofaustralia.net.au/home/species/4018</t>
+  </si>
+  <si>
+    <t>https://fishesofaustralia.net.au/images/image/StemonosudRothschildiCSIRO.jpg</t>
+  </si>
+  <si>
+    <t>Fishes of Australia</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Argentina_(fish)#/media/File:Atlantic_argentine_(_Argentina_silus_).jpg</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Atlantic_argentine_(_Argentina_silus_).jpg</t>
+  </si>
+  <si>
+    <t>https://www.sciencenews.org/wp-content/uploads/2015/02/wt_atlantic_cod_free.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t>Joachim S. M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ü</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ller</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/joachim_s_mueller/</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Clupea_harengus.png</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Jielbeaumadier_poisson_gris_2_paris_2014.jpeg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b6/Jielbeaumadier_poisson_gris_2_paris_2014.jpeg/800px-Jielbeaumadier_poisson_gris_2_paris_2014.jpeg</t>
+  </si>
+  <si>
+    <t>three-spine stickleback</t>
+  </si>
+  <si>
+    <t>Ryan Hagerty</t>
+  </si>
+  <si>
+    <t>https://nas.er.usgs.gov/queries/factsheet.aspx?SpeciesID=702</t>
+  </si>
+  <si>
+    <t>https://www.dfo-mpo.gc.ca/fisheries-peches/ifmp-gmp/capelin-area1-11-zone-capelan/img/capelin.jpg</t>
+  </si>
+  <si>
+    <t>Canadian Department of Fisheries and Oceans</t>
+  </si>
+  <si>
+    <t>https://www.dfo-mpo.gc.ca/fisheries-peches/ifmp-gmp/capelin-area1-11-zone-capelan/index-eng.html</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/proxy/UgD8LYjHL4_gs9itLt_1VcnG6rojPRGg-y0-MfFm7LGHr_qgvsdR7gRGYC0a8kpedc629nr19rIhB8_3LorYLJOoqSHvoa6z7ZhPdBf2bO9w8rRHEQREr1-oyfFpVyFvOOroHani16D-msQlVK1bvqYhuxdj9biGL5x0bHud2LnSZDqR2WwHwk9_iT96G6QK74B6N7OK8Za1XjSRm1Pi4AAlC49ygof7VgpaJcnGc4-Vf9A</t>
+  </si>
+  <si>
+    <t>http://www.invadingspecies.com/rainbow-smelt/#</t>
+  </si>
+  <si>
+    <t>Invading Species</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/physiology/FishSoundsSummary.php?autoctr=29</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/images/species/Mebil_u0.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +336,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -619,7 +688,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,10 +707,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -655,16 +724,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -678,16 +747,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -701,178 +770,232 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
+        <v>76</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -882,8 +1005,12 @@
     <hyperlink ref="B2" r:id="rId3" xr:uid="{3DEDF7B5-7AF5-42B1-96C5-B61C6B9D5CFB}"/>
     <hyperlink ref="G2" r:id="rId4" xr:uid="{6B23C7F8-DD8E-4996-939A-94246C59B42E}"/>
     <hyperlink ref="B3" r:id="rId5" xr:uid="{E63DF56C-245A-48AF-81A3-4014B3F250E3}"/>
+    <hyperlink ref="B5" r:id="rId6" location="/media/File:Atlantic_argentine_(_Argentina_silus_).jpg" xr:uid="{F9EB25DD-F124-4783-95E2-92F76FEC606F}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{CD088A44-CE79-4E40-A024-88F862213127}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{CFA1DB3B-A035-49AB-937F-727FC6242ED9}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{F919F405-B9CB-435B-B9D7-0F58493F79CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>